<commit_message>
A lot of comments/clarifications
Added my trace matrix and pseudocode
</commit_message>
<xml_diff>
--- a/Documentation/Trace Matrices/Dayton.xlsx
+++ b/Documentation/Trace Matrices/Dayton.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ALGONQUIN\UE\Team TeamTeam\TeamTeam\Documentation\Trace Matrices\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CB78860B-05A2-48D5-8A3B-C242E0EE3DF2}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1AC3761-6341-44F0-908B-67F0AE3BDBFE}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="60">
   <si>
     <t>Feature/User Story</t>
   </si>
@@ -129,15 +129,9 @@
     <t>Asset Fetching from GameMode</t>
   </si>
   <si>
-    <t>191-230</t>
-  </si>
-  <si>
     <t>Created Test room</t>
   </si>
   <si>
-    <t>../game/Blueprints/Test-Rooms</t>
-  </si>
-  <si>
     <t>BP_Test_Room_1.uasset</t>
   </si>
   <si>
@@ -147,15 +141,9 @@
     <t>Random Level Generation</t>
   </si>
   <si>
-    <t>96-160</t>
-  </si>
-  <si>
     <t>Load Assets into the GameMode for generation</t>
   </si>
   <si>
-    <t>16-74</t>
-  </si>
-  <si>
     <t>AssetTemplate.[cpp,h]</t>
   </si>
   <si>
@@ -190,6 +178,39 @@
   </si>
   <si>
     <t>UML.dia</t>
+  </si>
+  <si>
+    <t>16-100</t>
+  </si>
+  <si>
+    <t>116-191</t>
+  </si>
+  <si>
+    <t>240-270</t>
+  </si>
+  <si>
+    <t>../game/Blueprints/Test_Rooms</t>
+  </si>
+  <si>
+    <t>Documentation/Pseudocode</t>
+  </si>
+  <si>
+    <t>Pseudocode for above algorithms</t>
+  </si>
+  <si>
+    <t>Dayton - Pseudocode.docx</t>
+  </si>
+  <si>
+    <t>Code - WIP</t>
+  </si>
+  <si>
+    <t>RoomActorBase, LootingLootsGameModeBase, DoorActor, LootActor, AssetTemplate</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Attempted networking of level layout</t>
   </si>
 </sst>
 </file>
@@ -685,8 +706,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -843,7 +864,7 @@
     </row>
     <row r="8" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>26</v>
@@ -864,7 +885,7 @@
     </row>
     <row r="9" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>26</v>
@@ -885,7 +906,7 @@
     </row>
     <row r="10" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>26</v>
@@ -898,7 +919,7 @@
       </c>
       <c r="E10" s="3"/>
       <c r="F10" s="3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="G10" s="8" t="s">
         <v>17</v>
@@ -906,7 +927,7 @@
     </row>
     <row r="11" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>26</v>
@@ -922,12 +943,12 @@
         <v>30</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>26</v>
@@ -943,7 +964,7 @@
         <v>30</v>
       </c>
       <c r="G12" s="8" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -964,12 +985,12 @@
         <v>30</v>
       </c>
       <c r="G13" s="8" t="s">
-        <v>32</v>
+        <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>26</v>
@@ -978,19 +999,19 @@
         <v>15</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>34</v>
+        <v>52</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F14" s="3"/>
       <c r="G14" s="8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>26</v>
@@ -1003,48 +1024,72 @@
       </c>
       <c r="E15" s="3"/>
       <c r="F15" s="3" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="G15" s="8" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E16" s="3" t="s">
         <v>48</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>52</v>
       </c>
       <c r="F16" s="3"/>
       <c r="G16" s="8"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="7"/>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
+    <row r="17" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A17" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="F17" s="3"/>
-      <c r="G17" s="8"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="7"/>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
+      <c r="G17" s="8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+      <c r="A18" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>10</v>
+      </c>
       <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="8"/>
+      <c r="F18" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="G18" s="8" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="7"/>

</xml_diff>